<commit_message>
3.3.1.1 --> 3.4.0 update land/ICoLUPpUA (forest management cost from AFF)
</commit_message>
<xml_diff>
--- a/InputData/land/ICoLUPpUA/Impl Cost of Land Use Policies per Unit Area.xlsx
+++ b/InputData/land/ICoLUPpUA/Impl Cost of Land Use Policies per Unit Area.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\land\ICoLUPpUA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\land\ICoLUPpUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D03A0F-C9B7-42B1-BB63-04F4F1A0D5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB5B845-7794-4D4D-928D-785A12040715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38775" yWindow="5130" windowWidth="20625" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="100" windowWidth="16420" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,11 @@
   </sheets>
   <definedNames>
     <definedName name="C_to_CO2">44/12</definedName>
-    <definedName name="EUR2007_to_2012">About!$A$42</definedName>
-    <definedName name="EURtoUSD">About!$A$41</definedName>
-    <definedName name="ha_to_acre">About!$A$38</definedName>
-    <definedName name="USD1990_to_2012">About!$A$45</definedName>
-    <definedName name="USD1997_to_2012">About!$A$46</definedName>
+    <definedName name="EUR2007_to_2012">About!$A$38</definedName>
+    <definedName name="EURtoUSD">About!$A$37</definedName>
+    <definedName name="ha_to_acre">About!$A$34</definedName>
+    <definedName name="USD1990_to_2012">About!$A$41</definedName>
+    <definedName name="USD1997_to_2012">About!$A$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>ICoLUPpUA Implementation Cost of Land Use Policies per Unit Area</t>
   </si>
@@ -128,9 +128,6 @@
     <t>2012$ / acre / yr</t>
   </si>
   <si>
-    <t>Table 1</t>
-  </si>
-  <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
   </si>
   <si>
@@ -173,18 +170,6 @@
     <t>EUR/ha</t>
   </si>
   <si>
-    <t>Cost difference between active and passive forest management</t>
-  </si>
-  <si>
-    <t>U.S. Forest Service</t>
-  </si>
-  <si>
-    <t>Costs of Sequestering Carbon Through Tree Planting and Forest Management in the United States</t>
-  </si>
-  <si>
-    <t>https://archive.org/details/CAT91946672</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -228,6 +213,12 @@
   </si>
   <si>
     <t>acres in one hectare</t>
+  </si>
+  <si>
+    <t>Forest Management Costs</t>
+  </si>
+  <si>
+    <t>Consultation with American Forest Foundation</t>
   </si>
 </sst>
 </file>
@@ -369,7 +360,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -381,7 +372,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -728,230 +718,206 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="78.1328125" customWidth="1"/>
+    <col min="2" max="2" width="78.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2007</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2.47105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>1.2847999999999999</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1.7589999999999999</v>
+      </c>
+      <c r="B41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" s="3">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="B42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="3">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B23" s="6"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>2.47105</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>1.2847999999999999</v>
-      </c>
-      <c r="B41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>1.7589999999999999</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>1.4330000000000001</v>
-      </c>
-      <c r="B46" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -960,22 +926,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.3984375" customWidth="1"/>
+    <col min="1" max="1" width="39.36328125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -989,7 +957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1004,7 +972,7 @@
         <v>3.6999999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1019,7 +987,7 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1002,7 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1017,7 @@
         <v>2.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1064,7 +1032,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1079,7 +1047,7 @@
         <v>4.3999999999999986</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1094,7 +1062,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1109,7 +1077,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1124,7 +1092,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1139,12 +1107,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>AVERAGE(D3:D12)</f>
         <v>3.41</v>
@@ -1153,9 +1121,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
-        <f>A15*About!A45</f>
+        <f>A15*About!A41</f>
         <v>5.9981900000000001</v>
       </c>
       <c r="B16" t="s">
@@ -1173,20 +1141,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1194,13 +1162,13 @@
         <v>1550</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>2007</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1176,7 @@
         <v>1200</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>2012</v>
@@ -1226,20 +1194,22 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1256,16 +1226,16 @@
         <v>854.62186585130905</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <f>'Impr Forest Mgmt'!A16</f>
-        <v>5.9981900000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <f>25/1.5</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1282,7 +1252,7 @@
         <v>623.92909896602657</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>